<commit_message>
fix beeware-ext for 3.11
</commit_message>
<xml_diff>
--- a/source/projects/py/notes/builder/matrix.xlsx
+++ b/source/projects/py/notes/builder/matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sa/Downloads/projects/py-js/source/py/notes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sa/Downloads/projects/py-js/source/projects/py/notes/builder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6C4099-ED6F-704C-AC70-2D25ABFBD48D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12B1E8E-67E2-194C-BB68-C357063056EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="3800" windowWidth="15660" windowHeight="11380" xr2:uid="{656454C3-FA4A-114C-8459-B2A646AF5476}"/>
+    <workbookView xWindow="860" yWindow="3800" windowWidth="25240" windowHeight="13240" activeTab="1" xr2:uid="{656454C3-FA4A-114C-8459-B2A646AF5476}"/>
   </bookViews>
   <sheets>
     <sheet name="testing" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="67">
   <si>
     <t>static</t>
   </si>
@@ -102,18 +102,6 @@
     <t>xcode_proj</t>
   </si>
   <si>
-    <t>bin-homebrew-sys</t>
-  </si>
-  <si>
-    <t>bin-homebrew-ext</t>
-  </si>
-  <si>
-    <t>bin-homebrew-pkg</t>
-  </si>
-  <si>
-    <t>src-static-ext</t>
-  </si>
-  <si>
     <t>static-ext</t>
   </si>
   <si>
@@ -135,30 +123,12 @@
     <t>depends_on</t>
   </si>
   <si>
-    <t>src-shared-ext</t>
-  </si>
-  <si>
-    <t>src-shared-pkg</t>
-  </si>
-  <si>
     <t>py-js build variations 0.1.1</t>
   </si>
   <si>
     <t>relocatable-pkg</t>
   </si>
   <si>
-    <t>src-framework-ext</t>
-  </si>
-  <si>
-    <t>src-framework-pkg</t>
-  </si>
-  <si>
-    <t>src-shared-pkg-rpath</t>
-  </si>
-  <si>
-    <t>src-static-pkg</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
@@ -262,6 +232,12 @@
   </si>
   <si>
     <t>[2]</t>
+  </si>
+  <si>
+    <t>local-sys</t>
+  </si>
+  <si>
+    <t>static-pkg</t>
   </si>
 </sst>
 </file>
@@ -319,7 +295,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,12 +311,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -456,58 +426,52 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -525,16 +489,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -850,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C7EDD8-2303-1D4E-BD35-415BCD4B1B09}">
   <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -861,33 +815,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="C2" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="C2" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>70</v>
+      <c r="B3" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
@@ -904,7 +858,7 @@
     </row>
     <row r="5" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -913,12 +867,12 @@
       </c>
       <c r="F5" s="5"/>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -927,12 +881,12 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -949,7 +903,7 @@
     </row>
     <row r="8" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -966,7 +920,7 @@
     </row>
     <row r="9" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -983,7 +937,7 @@
     </row>
     <row r="10" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1000,7 +954,7 @@
     </row>
     <row r="11" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
@@ -1017,7 +971,7 @@
     </row>
     <row r="12" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1026,12 +980,12 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -1047,7 +1001,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B16" s="32"/>
+      <c r="B16" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1072,8 +1026,8 @@
   </sheetPr>
   <dimension ref="B1:N21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1093,7 +1047,7 @@
   <sheetData>
     <row r="1" spans="2:14" ht="24" x14ac:dyDescent="0.3">
       <c r="B1" s="11" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="19" x14ac:dyDescent="0.25">
@@ -1107,7 +1061,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>20</v>
@@ -1119,13 +1073,13 @@
         <v>4</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>15</v>
@@ -1138,8 +1092,8 @@
       </c>
     </row>
     <row r="4" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
-        <v>56</v>
+      <c r="B4" s="28" t="s">
+        <v>46</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>17</v>
@@ -1147,11 +1101,11 @@
       <c r="D4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>53</v>
+      <c r="E4" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>43</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>2</v>
@@ -1179,15 +1133,15 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B5" s="21"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1214,8 +1168,8 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
-        <v>57</v>
+      <c r="B6" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>17</v>
@@ -1223,11 +1177,11 @@
       <c r="D6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="26" t="s">
         <v>44</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>54</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>2</v>
@@ -1255,15 +1209,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B7" s="21"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="5" t="s">
         <v>3</v>
       </c>
@@ -1290,8 +1244,8 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
-        <v>58</v>
+      <c r="B8" s="28" t="s">
+        <v>48</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>17</v>
@@ -1299,11 +1253,11 @@
       <c r="D8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>55</v>
+      <c r="E8" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>2</v>
@@ -1314,7 +1268,7 @@
       <c r="I8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="17">
         <v>1</v>
       </c>
       <c r="K8" s="5">
@@ -1326,20 +1280,20 @@
       <c r="M8" s="5">
         <v>1</v>
       </c>
-      <c r="N8" s="22">
+      <c r="N8" s="29">
         <v>13.9</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B9" s="21"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="5" t="s">
         <v>3</v>
       </c>
@@ -1349,7 +1303,7 @@
       <c r="I9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="17">
         <v>1</v>
       </c>
       <c r="K9" s="5">
@@ -1361,11 +1315,11 @@
       <c r="M9" s="5">
         <v>1</v>
       </c>
-      <c r="N9" s="22"/>
+      <c r="N9" s="29"/>
     </row>
     <row r="10" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
-        <v>59</v>
+      <c r="B10" s="28" t="s">
+        <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>18</v>
@@ -1373,11 +1327,11 @@
       <c r="D10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>25</v>
+      <c r="E10" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>21</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>2</v>
@@ -1405,15 +1359,15 @@
       </c>
     </row>
     <row r="11" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B11" s="21"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="G11" s="5" t="s">
         <v>3</v>
       </c>
@@ -1440,8 +1394,8 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
-        <v>60</v>
+      <c r="B12" s="28" t="s">
+        <v>50</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>18</v>
@@ -1449,11 +1403,11 @@
       <c r="D12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>26</v>
+      <c r="E12" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>2</v>
@@ -1481,15 +1435,15 @@
       </c>
     </row>
     <row r="13" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B13" s="21"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="5" t="s">
         <v>3</v>
       </c>
@@ -1516,8 +1470,8 @@
       </c>
     </row>
     <row r="14" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
-        <v>61</v>
+      <c r="B14" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>18</v>
@@ -1525,11 +1479,11 @@
       <c r="D14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>27</v>
+      <c r="E14" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>23</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>2</v>
@@ -1557,15 +1511,15 @@
       </c>
     </row>
     <row r="15" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B15" s="21"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="5" t="s">
         <v>3</v>
       </c>
@@ -1592,8 +1546,8 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
-        <v>62</v>
+      <c r="B16" s="28" t="s">
+        <v>52</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>18</v>
@@ -1601,11 +1555,11 @@
       <c r="D16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>28</v>
+      <c r="E16" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>24</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>2</v>
@@ -1628,21 +1582,21 @@
       <c r="M16" s="5">
         <v>1</v>
       </c>
-      <c r="N16" s="22">
+      <c r="N16" s="29">
         <f>18.7</f>
         <v>18.7</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B17" s="21"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
       <c r="G17" s="5" t="s">
         <v>3</v>
       </c>
@@ -1664,21 +1618,21 @@
       <c r="M17" s="5">
         <v>1</v>
       </c>
-      <c r="N17" s="22"/>
+      <c r="N17" s="29"/>
     </row>
     <row r="18" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B18" s="23" t="s">
-        <v>63</v>
+      <c r="B18" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="13"/>
-      <c r="E18" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="26" t="s">
-        <v>29</v>
+      <c r="E18" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>2</v>
@@ -1702,13 +1656,13 @@
       <c r="N18" s="10"/>
     </row>
     <row r="19" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B19" s="23"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="13"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="9" t="s">
         <v>3</v>
       </c>
@@ -1731,8 +1685,8 @@
       <c r="N19" s="10"/>
     </row>
     <row r="20" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
-        <v>64</v>
+      <c r="B20" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>18</v>
@@ -1740,11 +1694,11 @@
       <c r="D20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>30</v>
+      <c r="E20" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>2</v>
@@ -1767,18 +1721,18 @@
       <c r="M20" s="9">
         <v>1</v>
       </c>
-      <c r="N20" s="28"/>
+      <c r="N20" s="25"/>
     </row>
     <row r="21" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B21" s="23"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="9" t="s">
         <v>3</v>
       </c>
@@ -1800,10 +1754,24 @@
       <c r="M21" s="9">
         <v>1</v>
       </c>
-      <c r="N21" s="28"/>
+      <c r="N21" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="N20:N21"/>
@@ -1820,20 +1788,6 @@
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="58" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -1842,10 +1796,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C27982-693A-F04A-877F-4F325C25078C}">
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:E21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1858,22 +1812,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>45</v>
+      <c r="B2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="15" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="15"/>
@@ -1881,7 +1835,7 @@
     </row>
     <row r="4" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="15" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="15"/>
@@ -1889,39 +1843,36 @@
     </row>
     <row r="5" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
     </row>
     <row r="6" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="14"/>
-      <c r="C6" s="16" t="s">
-        <v>29</v>
+      <c r="B6" s="30" t="s">
+        <v>25</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
     </row>
     <row r="7" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="14"/>
-      <c r="C7" s="16" t="s">
-        <v>30</v>
+      <c r="B7" s="30" t="s">
+        <v>26</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
     </row>
     <row r="8" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="14"/>
+      <c r="B8" s="30" t="s">
+        <v>29</v>
+      </c>
       <c r="C8" s="14"/>
-      <c r="D8" s="17" t="s">
-        <v>35</v>
-      </c>
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="15"/>
@@ -1929,87 +1880,85 @@
     </row>
     <row r="10" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
     </row>
     <row r="11" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="14"/>
+      <c r="B11" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="19" t="s">
-        <v>36</v>
-      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
     </row>
     <row r="12" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="14"/>
+      <c r="B12" s="15" t="s">
+        <v>66</v>
+      </c>
       <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="19" t="s">
-        <v>37</v>
-      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="15"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15" t="s">
-        <v>32</v>
-      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="15"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="14"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="14"/>
-      <c r="D15" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
       <c r="C16" s="14"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15" t="s">
-        <v>24</v>
-      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
-      <c r="D17" s="17" t="s">
-        <v>39</v>
-      </c>
+      <c r="D17" s="14"/>
       <c r="E17" s="14"/>
     </row>
     <row r="18" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="15" t="s">
-        <v>25</v>
-      </c>
+      <c r="B18" s="15"/>
       <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="B19" s="15" t="s">
-        <v>26</v>
-      </c>
+    <row r="19" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="14"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="15"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="2:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="B21" s="15"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:B19">
-    <sortCondition ref="B3:B19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:B21">
+    <sortCondition ref="B3:B21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>